<commit_message>
try 2 to get data
try 2 to get data
</commit_message>
<xml_diff>
--- a/ProjectExcelsAndData/GExtensions.xlsx
+++ b/ProjectExcelsAndData/GExtensions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Akbar Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
   <si>
     <t xml:space="preserve">Data To Be Caputred </t>
   </si>
@@ -112,27 +112,9 @@
     <t>Airline_PNR</t>
   </si>
   <si>
-    <t>$(".referenceno &gt; a").text()</t>
-  </si>
-  <si>
-    <t>$(".mainheadright &gt; .headernav").text()</t>
-  </si>
-  <si>
-    <t>$(".airline &gt; .item:eq(0)").text()</t>
-  </si>
-  <si>
-    <t>$(".flighttype").attr("title")</t>
-  </si>
-  <si>
-    <t>$(".refund").attr("title")</t>
-  </si>
-  <si>
     <t>Airline_FlightType</t>
   </si>
   <si>
-    <t>$(".airline &gt; .item:eq(1)").text()</t>
-  </si>
-  <si>
     <r>
       <t>$</t>
     </r>
@@ -611,6 +593,48 @@
       </rPr>
       <t>()</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">var _Referenceno </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $(".referenceno &gt; strong &gt; a").text(); </t>
+  </si>
+  <si>
+    <t xml:space="preserve">var _PNRNo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $(_MainParent).find('.itemheadersub &gt; .mainheadright &gt; .headernav:eq(0)').text().split("|")[1].split(":")[1];</t>
+  </si>
+  <si>
+    <t xml:space="preserve">var _AirlineID </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $(_MainParent).find('.airline &gt; .item:eq(1)').html().split("&lt;br&gt;")[0];</t>
+  </si>
+  <si>
+    <t xml:space="preserve">var _AirlineName </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $(_MainParent).find(".airline &gt; .item:eq(1)").html().split("&lt;br&gt;")[1];</t>
+  </si>
+  <si>
+    <t xml:space="preserve">var _Refund </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $(_MainParent).find(".refund").attr("title");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">var _FlightType </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $(_MainParent).find(".flighttype").attr("title");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">var _BookingType </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $(_MainParent).find(".airline &gt; .item:eq(2)").text();</t>
   </si>
 </sst>
 </file>
@@ -695,8 +719,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -980,14 +1004,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.7109375" customWidth="1"/>
+    <col min="2" max="2" width="68.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.140625" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
@@ -1024,8 +1048,8 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>30</v>
+      <c r="B2" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -1043,12 +1067,12 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>31</v>
+      <c r="B3" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
@@ -1069,8 +1093,8 @@
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>32</v>
+      <c r="B4" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -1091,8 +1115,8 @@
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>32</v>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1109,8 +1133,8 @@
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>34</v>
+      <c r="B6" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -1125,10 +1149,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1145,8 +1169,8 @@
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>36</v>
+      <c r="B8" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1382,20 +1406,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="145" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>37</v>
+      <c r="A1" t="s">
+        <v>31</v>
       </c>
       <c r="B1" t="str">
         <f>"console.log("&amp;A1&amp;");"</f>
@@ -1403,8 +1428,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>38</v>
+      <c r="A2" t="s">
+        <v>32</v>
       </c>
       <c r="B2" t="str">
         <f t="shared" ref="B2:B7" si="0">"console.log("&amp;A2&amp;");"</f>
@@ -1412,8 +1437,8 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>39</v>
+      <c r="A3" t="s">
+        <v>33</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" si="0"/>
@@ -1421,8 +1446,8 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>39</v>
+      <c r="A4" t="s">
+        <v>33</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
@@ -1430,8 +1455,8 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>40</v>
+      <c r="A5" t="s">
+        <v>34</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
@@ -1439,8 +1464,8 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>41</v>
+      <c r="A6" t="s">
+        <v>35</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
@@ -1448,15 +1473,51 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>42</v>
+      <c r="A7" t="s">
+        <v>36</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
         <v>console.log($(".airline &gt; .item:eq(1)").text());</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed Passenger & Airline Data
Completed Passenger & Airline Data
</commit_message>
<xml_diff>
--- a/ProjectExcelsAndData/GExtensions.xlsx
+++ b/ProjectExcelsAndData/GExtensions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
   <si>
     <t xml:space="preserve">Data To Be Caputred </t>
   </si>
@@ -635,6 +635,9 @@
   </si>
   <si>
     <t xml:space="preserve"> $(_MainParent).find(".airline &gt; .item:eq(2)").text();</t>
+  </si>
+  <si>
+    <t>Duration_Time</t>
   </si>
 </sst>
 </file>
@@ -1004,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,7 +1085,9 @@
         <v>10</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>

</xml_diff>